<commit_message>
fixed so recaptcha works and alert on submit
</commit_message>
<xml_diff>
--- a/littlethings.xlsx
+++ b/littlethings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github\littleThings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C0914F-DAF3-4DE2-B80C-0B804191D98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE3F490-B051-4ABF-ABE5-6F36FE89BC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF20BAB8-ACE3-4EA9-B65E-CC28FD72C416}"/>
   </bookViews>
@@ -21,7 +21,6 @@
     <definedName name="ExternalData_3" localSheetId="0" hidden="1">Table1_3!$A$1:$B$163</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="199">
   <si>
     <t>Column1</t>
   </si>
@@ -638,6 +637,21 @@
   </si>
   <si>
     <t>('moisturizing cream'),</t>
+  </si>
+  <si>
+    <t>new stuff</t>
+  </si>
+  <si>
+    <t>input already</t>
+  </si>
+  <si>
+    <t>pizza and fries</t>
+  </si>
+  <si>
+    <t>running water</t>
+  </si>
+  <si>
+    <t>a good night's sleep</t>
   </si>
 </sst>
 </file>
@@ -673,9 +687,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,8 +745,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{201AF3D2-ADB7-4D5E-845F-004EDE1A5E8D}" name="Table1_4" displayName="Table1_4" ref="A1:B163" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B163" xr:uid="{201AF3D2-ADB7-4D5E-845F-004EDE1A5E8D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7606B0E5-5248-45CC-9955-470796298DD6}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{1F462154-B604-412E-B674-C3C2DB0979F5}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7606B0E5-5248-45CC-9955-470796298DD6}" uniqueName="1" name="input already" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{1F462154-B604-412E-B674-C3C2DB0979F5}" uniqueName="2" name="new stuff" queryTableFieldId="2" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -743,8 +756,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7E4F6036-8A6A-4DB9-9081-1D0CF411FEE7}" name="Table1_3" displayName="Table1_3" ref="A1:B133" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B133" xr:uid="{7E4F6036-8A6A-4DB9-9081-1D0CF411FEE7}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{44AE1181-9A8D-4647-B76D-55E4A5E183FE}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{E1BAE5BF-92BD-454D-8BAC-DE6035619EC0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{44AE1181-9A8D-4647-B76D-55E4A5E183FE}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E1BAE5BF-92BD-454D-8BAC-DE6035619EC0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1050,7 +1063,7 @@
   <dimension ref="A1:B163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,953 +1074,830 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>31</v>
       </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>34</v>
       </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>21</v>
       </c>
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>46</v>
       </c>
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>23</v>
       </c>
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>82</v>
       </c>
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>44</v>
       </c>
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>25</v>
       </c>
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>43</v>
       </c>
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>26</v>
       </c>
-      <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>27</v>
       </c>
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>42</v>
       </c>
-      <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>41</v>
       </c>
-      <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>76</v>
       </c>
-      <c r="B66" s="1"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>28</v>
       </c>
-      <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>67</v>
       </c>
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>66</v>
       </c>
-      <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>68</v>
       </c>
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>72</v>
       </c>
-      <c r="B76" s="1"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>73</v>
       </c>
-      <c r="B77" s="1"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>74</v>
       </c>
-      <c r="B78" s="1"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>75</v>
       </c>
-      <c r="B79" s="1"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>77</v>
       </c>
-      <c r="B80" s="1"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>78</v>
       </c>
-      <c r="B81" s="1"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>79</v>
       </c>
-      <c r="B82" s="1"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>80</v>
       </c>
-      <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>81</v>
       </c>
-      <c r="B84" s="1"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>83</v>
       </c>
-      <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>84</v>
       </c>
-      <c r="B86" s="1"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="B87" s="1"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>88</v>
       </c>
-      <c r="B90" s="1"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="1"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B92" s="1"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>91</v>
       </c>
-      <c r="B93" s="1"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>92</v>
       </c>
-      <c r="B94" s="1"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>93</v>
       </c>
-      <c r="B95" s="1"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>94</v>
       </c>
-      <c r="B96" s="1"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>95</v>
       </c>
-      <c r="B97" s="1"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>96</v>
       </c>
-      <c r="B98" s="1"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>97</v>
       </c>
-      <c r="B99" s="1"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>98</v>
       </c>
-      <c r="B100" s="1"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="1"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="1"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="1"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>105</v>
       </c>
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="1"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>107</v>
       </c>
-      <c r="B107" s="1"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>108</v>
       </c>
-      <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>109</v>
       </c>
-      <c r="B109" s="1"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>110</v>
       </c>
-      <c r="B110" s="1"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>111</v>
       </c>
-      <c r="B111" s="1"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>112</v>
       </c>
-      <c r="B112" s="1"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>113</v>
       </c>
-      <c r="B113" s="1"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>114</v>
       </c>
-      <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>115</v>
       </c>
-      <c r="B115" s="1"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>116</v>
       </c>
-      <c r="B116" s="1"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>117</v>
       </c>
-      <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>118</v>
       </c>
-      <c r="B118" s="1"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>119</v>
       </c>
-      <c r="B119" s="1"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>120</v>
       </c>
-      <c r="B120" s="1"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>121</v>
       </c>
-      <c r="B121" s="1"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>122</v>
       </c>
-      <c r="B122" s="1"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>123</v>
       </c>
-      <c r="B123" s="1"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
         <v>124</v>
       </c>
-      <c r="B124" s="1"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>125</v>
       </c>
-      <c r="B125" s="1"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>126</v>
       </c>
-      <c r="B126" s="1"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>127</v>
       </c>
-      <c r="B127" s="1"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>128</v>
       </c>
-      <c r="B128" s="1"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>129</v>
       </c>
-      <c r="B129" s="1"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>130</v>
       </c>
-      <c r="B130" s="1"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="1" t="s">
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>131</v>
       </c>
-      <c r="B131" s="1"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>132</v>
       </c>
-      <c r="B132" s="1"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>133</v>
       </c>
-      <c r="B133" s="1"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>164</v>
       </c>
-      <c r="B134" s="1"/>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
         <v>165</v>
       </c>
-      <c r="B135" s="1"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>166</v>
       </c>
-      <c r="B136" s="1"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="1" t="s">
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>167</v>
       </c>
-      <c r="B137" s="1"/>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>168</v>
       </c>
-      <c r="B138" s="1"/>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="1" t="s">
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>169</v>
       </c>
-      <c r="B139" s="1"/>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="1" t="s">
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
         <v>170</v>
       </c>
-      <c r="B140" s="1"/>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="1" t="s">
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
         <v>171</v>
       </c>
-      <c r="B141" s="1"/>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="1" t="s">
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>172</v>
       </c>
-      <c r="B142" s="1"/>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="1" t="s">
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
         <v>173</v>
       </c>
-      <c r="B143" s="1"/>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="1" t="s">
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
         <v>174</v>
       </c>
-      <c r="B144" s="1"/>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="1" t="s">
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
         <v>175</v>
       </c>
-      <c r="B145" s="1"/>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="1" t="s">
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>176</v>
       </c>
-      <c r="B146" s="1"/>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="1" t="s">
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
         <v>177</v>
       </c>
-      <c r="B147" s="1"/>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="1" t="s">
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
         <v>178</v>
       </c>
-      <c r="B148" s="1"/>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="1" t="s">
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
         <v>179</v>
       </c>
-      <c r="B149" s="1"/>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="1" t="s">
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
         <v>180</v>
       </c>
-      <c r="B150" s="1"/>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="1" t="s">
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
         <v>181</v>
       </c>
-      <c r="B151" s="1"/>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="1" t="s">
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
         <v>182</v>
       </c>
-      <c r="B152" s="1"/>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="1" t="s">
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
         <v>183</v>
       </c>
-      <c r="B153" s="1"/>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="1" t="s">
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
         <v>184</v>
       </c>
-      <c r="B154" s="1"/>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="1" t="s">
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
         <v>185</v>
       </c>
-      <c r="B155" s="1"/>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="1" t="s">
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
         <v>186</v>
       </c>
-      <c r="B156" s="1"/>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="1" t="s">
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
         <v>187</v>
       </c>
-      <c r="B157" s="1"/>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="1" t="s">
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
         <v>188</v>
       </c>
-      <c r="B158" s="1"/>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" s="1" t="s">
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
         <v>189</v>
       </c>
-      <c r="B159" s="1"/>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="1" t="s">
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
         <v>190</v>
       </c>
-      <c r="B160" s="1"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="1" t="s">
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
         <v>191</v>
       </c>
-      <c r="B161" s="1"/>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="1" t="s">
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
         <v>192</v>
       </c>
-      <c r="B162" s="1"/>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="1" t="s">
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
         <v>193</v>
       </c>
-      <c r="B163" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2022,7 +1912,7 @@
   <dimension ref="A1:B133"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B31"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2040,7 +1930,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
@@ -2048,7 +1938,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
       <c r="B3" t="s">
@@ -2056,7 +1946,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4" t="s">
@@ -2064,7 +1954,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
@@ -2072,7 +1962,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>61</v>
       </c>
       <c r="B6" t="s">
@@ -2080,7 +1970,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
       <c r="B7" t="s">
@@ -2088,7 +1978,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>37</v>
       </c>
       <c r="B8" t="s">
@@ -2096,7 +1986,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>38</v>
       </c>
       <c r="B9" t="s">
@@ -2104,7 +1994,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
@@ -2112,7 +2002,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
@@ -2120,7 +2010,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>39</v>
       </c>
       <c r="B12" t="s">
@@ -2128,7 +2018,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>57</v>
       </c>
       <c r="B13" t="s">
@@ -2136,7 +2026,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
@@ -2144,7 +2034,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>56</v>
       </c>
       <c r="B15" t="s">
@@ -2152,7 +2042,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>54</v>
       </c>
       <c r="B16" t="s">
@@ -2160,7 +2050,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>55</v>
       </c>
       <c r="B17" t="s">
@@ -2168,7 +2058,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>40</v>
       </c>
       <c r="B18" t="s">
@@ -2176,7 +2066,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19" t="s">
@@ -2184,7 +2074,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20" t="s">
@@ -2192,7 +2082,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" t="s">
@@ -2200,7 +2090,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>64</v>
       </c>
       <c r="B22" t="s">
@@ -2208,7 +2098,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" t="s">
@@ -2216,7 +2106,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>99</v>
       </c>
       <c r="B24" t="s">
@@ -2224,7 +2114,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="B25" t="s">
@@ -2232,7 +2122,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="B26" t="s">
@@ -2240,7 +2130,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>10</v>
       </c>
       <c r="B27" t="s">
@@ -2248,7 +2138,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" t="s">
@@ -2256,7 +2146,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29" t="s">
@@ -2264,7 +2154,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30" t="s">
@@ -2272,624 +2162,522 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>21</v>
       </c>
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>46</v>
       </c>
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>23</v>
       </c>
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>82</v>
       </c>
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>44</v>
       </c>
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>25</v>
       </c>
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>43</v>
       </c>
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>26</v>
       </c>
-      <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>27</v>
       </c>
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>42</v>
       </c>
-      <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>41</v>
       </c>
-      <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>76</v>
       </c>
-      <c r="B66" s="1"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>28</v>
       </c>
-      <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>67</v>
       </c>
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>66</v>
       </c>
-      <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>68</v>
       </c>
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>72</v>
       </c>
-      <c r="B76" s="1"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>73</v>
       </c>
-      <c r="B77" s="1"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>74</v>
       </c>
-      <c r="B78" s="1"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>75</v>
       </c>
-      <c r="B79" s="1"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>77</v>
       </c>
-      <c r="B80" s="1"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>78</v>
       </c>
-      <c r="B81" s="1"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>79</v>
       </c>
-      <c r="B82" s="1"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>80</v>
       </c>
-      <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>81</v>
       </c>
-      <c r="B84" s="1"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>83</v>
       </c>
-      <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>84</v>
       </c>
-      <c r="B86" s="1"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="B87" s="1"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>88</v>
       </c>
-      <c r="B90" s="1"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="1"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B92" s="1"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>91</v>
       </c>
-      <c r="B93" s="1"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>92</v>
       </c>
-      <c r="B94" s="1"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>93</v>
       </c>
-      <c r="B95" s="1"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>94</v>
       </c>
-      <c r="B96" s="1"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>95</v>
       </c>
-      <c r="B97" s="1"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>96</v>
       </c>
-      <c r="B98" s="1"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>97</v>
       </c>
-      <c r="B99" s="1"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>98</v>
       </c>
-      <c r="B100" s="1"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="1"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="1"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="1"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>105</v>
       </c>
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="1"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>107</v>
       </c>
-      <c r="B107" s="1"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>108</v>
       </c>
-      <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>109</v>
       </c>
-      <c r="B109" s="1"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>110</v>
       </c>
-      <c r="B110" s="1"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>111</v>
       </c>
-      <c r="B111" s="1"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>112</v>
       </c>
-      <c r="B112" s="1"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>113</v>
       </c>
-      <c r="B113" s="1"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>114</v>
       </c>
-      <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>115</v>
       </c>
-      <c r="B115" s="1"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>116</v>
       </c>
-      <c r="B116" s="1"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>117</v>
       </c>
-      <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>118</v>
       </c>
-      <c r="B118" s="1"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>119</v>
       </c>
-      <c r="B119" s="1"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>120</v>
       </c>
-      <c r="B120" s="1"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>121</v>
       </c>
-      <c r="B121" s="1"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>122</v>
       </c>
-      <c r="B122" s="1"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>123</v>
       </c>
-      <c r="B123" s="1"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
         <v>124</v>
       </c>
-      <c r="B124" s="1"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>125</v>
       </c>
-      <c r="B125" s="1"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>126</v>
       </c>
-      <c r="B126" s="1"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>127</v>
       </c>
-      <c r="B127" s="1"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>128</v>
       </c>
-      <c r="B128" s="1"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>129</v>
       </c>
-      <c r="B129" s="1"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>130</v>
       </c>
-      <c r="B130" s="1"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="1" t="s">
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>131</v>
       </c>
-      <c r="B131" s="1"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>132</v>
       </c>
-      <c r="B132" s="1"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>133</v>
       </c>
-      <c r="B133" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed some stuff, fixed other stuff.
</commit_message>
<xml_diff>
--- a/littlethings.xlsx
+++ b/littlethings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github\littleThings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE3F490-B051-4ABF-ABE5-6F36FE89BC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EEA780-20D6-430B-8BFE-02495453B284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF20BAB8-ACE3-4EA9-B65E-CC28FD72C416}"/>
+    <workbookView xWindow="5760" yWindow="12" windowWidth="17280" windowHeight="8964" xr2:uid="{AF20BAB8-ACE3-4EA9-B65E-CC28FD72C416}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1_3" sheetId="4" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="203">
   <si>
     <t>Column1</t>
   </si>
@@ -652,6 +652,18 @@
   </si>
   <si>
     <t>a good night's sleep</t>
+  </si>
+  <si>
+    <t>firm mattresses</t>
+  </si>
+  <si>
+    <t>soft vanilla ice cream</t>
+  </si>
+  <si>
+    <t>potato peelers</t>
+  </si>
+  <si>
+    <t>an empty inbox</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1075,7 @@
   <dimension ref="A1:B163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1108,25 +1120,40 @@
       <c r="A5" t="s">
         <v>35</v>
       </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>61</v>
       </c>
+      <c r="B6" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
+      <c r="B7" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
+      <c r="B8" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>